<commit_message>
Try running with manual experiments:
THIS IS A BREAKING CHANGE

Details:
    * successfully use regex in get_explicit_experiments
    * filter is now optional in get_explicit_experiments
    * update MIT_PVLab_Template to use manually defined experiments
    * ermmoldf and manualmmoldf are conflicting
</commit_message>
<xml_diff>
--- a/MIT_PVLab_Template.xlsx
+++ b/MIT_PVLab_Template.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="233">
   <si>
     <t>Comment</t>
   </si>
@@ -1176,6 +1176,15 @@
   <si>
     <t>Manual Well Custom ID</t>
   </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>baz</t>
+  </si>
 </sst>
 </file>
 
@@ -2161,7 +2170,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2714,9 +2723,11 @@
       <c r="C16" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="45"/>
+      <c r="D16" s="45" t="s">
+        <v>2</v>
+      </c>
       <c r="E16" s="46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F16" s="47">
         <v>12</v>
@@ -14315,10 +14326,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K500"/>
+  <dimension ref="A1:T500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14366,11 +14377,13 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="91" t="str">
+      <c r="A2" s="91">
         <f>IF(manual_wells &gt; 0, 1, "")</f>
-        <v/>
-      </c>
-      <c r="B2" s="91"/>
+        <v>1</v>
+      </c>
+      <c r="B2" s="91" t="s">
+        <v>230</v>
+      </c>
       <c r="C2" s="90">
         <v>150</v>
       </c>
@@ -14395,17 +14408,19 @@
       <c r="J2" s="90">
         <v>0</v>
       </c>
-      <c r="K2" s="90" t="str">
+      <c r="K2" s="90">
         <f>IF(NOT(A2=""), SUM(C2:J2), "")</f>
-        <v/>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="91" t="str">
+      <c r="A3" s="91">
         <f>IF(A2 &lt; fixed_wells, A2 + 1, "")</f>
-        <v/>
-      </c>
-      <c r="B3" s="91"/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="91" t="s">
+        <v>231</v>
+      </c>
       <c r="C3" s="90">
         <v>150</v>
       </c>
@@ -14430,17 +14445,19 @@
       <c r="J3" s="90">
         <v>0</v>
       </c>
-      <c r="K3" s="90" t="str">
+      <c r="K3" s="90">
         <f t="shared" ref="K3:K66" si="0">IF(NOT(A3=""), SUM(C3:J3), "")</f>
-        <v/>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="91" t="str">
+      <c r="A4" s="91">
         <f t="shared" ref="A4:A34" si="1">IF(A3 &lt; fixed_wells, A3 + 1, "")</f>
-        <v/>
-      </c>
-      <c r="B4" s="91"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="91" t="s">
+        <v>232</v>
+      </c>
       <c r="C4" s="90">
         <v>150</v>
       </c>
@@ -14465,9 +14482,9 @@
       <c r="J4" s="90">
         <v>0</v>
       </c>
-      <c r="K4" s="90" t="str">
+      <c r="K4" s="90">
         <f t="shared" si="0"/>
-        <v/>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
@@ -14602,7 +14619,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14613,18 +14630,18 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="B18" s="91"/>
-      <c r="K18" s="90" t="str">
-        <f t="shared" si="0"/>
+      <c r="T18" s="90" t="str">
+        <f>IF(NOT(A18=""), SUM(C18:S18), "")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14635,7 +14652,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14646,7 +14663,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14657,7 +14674,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14668,7 +14685,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14679,7 +14696,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14690,7 +14707,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14701,7 +14718,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14712,7 +14729,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14723,7 +14740,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14734,7 +14751,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14745,7 +14762,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14756,7 +14773,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -14767,7 +14784,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" s="90" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="91" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -15900,7 +15917,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <ignoredErrors>
-    <ignoredError sqref="K2:K3 K4:K97" unlockedFormula="1"/>
+    <ignoredError sqref="T18 K2:K17 K19:K97" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -15910,7 +15927,7 @@
   <dimension ref="A1:W996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16410,7 +16427,7 @@
       <c r="C16" s="45"/>
       <c r="D16" s="34">
         <f>'User Interface'!E16</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E16" s="45" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
refact gettsheettarget into smaller funcitons: * get_observation_interface_uid * get_gdrive_client
</commit_message>
<xml_diff>
--- a/MIT_PVLab_Template.xlsx
+++ b/MIT_PVLab_Template.xlsx
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>exp1_vols</t>
-  </si>
-  <si>
-    <t>[[500,500]]</t>
   </si>
   <si>
     <t xml:space="preserve">Min and Max volumes for each portion of the experiment. </t>
@@ -1175,9 +1172,6 @@
     <t>Precursor3 (ul)</t>
   </si>
   <si>
-    <t>Precurso4 (ul)</t>
-  </si>
-  <si>
     <t>Precursor5 (ul)</t>
   </si>
   <si>
@@ -1226,7 +1220,13 @@
     <t>exp2_name</t>
   </si>
   <si>
-    <t>[[3,1]]</t>
+    <t>Precursor4 (ul)</t>
+  </si>
+  <si>
+    <t>[[2,3,1,]]</t>
+  </si>
+  <si>
+    <t>[[215, 215]]</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1820,6 +1820,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2212,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2306,7 +2309,7 @@
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="92" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D3" s="93" t="s">
         <v>2</v>
@@ -2318,7 +2321,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="13"/>
@@ -2350,16 +2353,16 @@
         <v>2</v>
       </c>
       <c r="E4" s="94" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>165</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -2414,7 +2417,7 @@
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>2</v>
@@ -2448,7 +2451,7 @@
     </row>
     <row r="7" spans="1:26" s="32" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="105" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="27"/>
@@ -2482,16 +2485,16 @@
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D8" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G8" s="36" t="s">
         <v>23</v>
@@ -2522,22 +2525,22 @@
       <c r="A9" s="33"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D9" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G9" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="37" t="s">
         <v>27</v>
-      </c>
-      <c r="H9" s="37" t="s">
-        <v>28</v>
       </c>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
@@ -2562,7 +2565,7 @@
       <c r="A10" s="33"/>
       <c r="B10" s="33"/>
       <c r="C10" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D10" s="35" t="s">
         <v>2</v>
@@ -2574,10 +2577,10 @@
         <v>12</v>
       </c>
       <c r="G10" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="37" t="s">
         <v>30</v>
-      </c>
-      <c r="H10" s="37" t="s">
-        <v>31</v>
       </c>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
@@ -2602,13 +2605,13 @@
       <c r="A11" s="33"/>
       <c r="B11" s="33"/>
       <c r="C11" s="34" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D11" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="36"/>
@@ -2633,8 +2636,8 @@
       <c r="Z11" s="38"/>
     </row>
     <row r="12" spans="1:26" s="32" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="116" t="s">
-        <v>225</v>
+      <c r="A12" s="117" t="s">
+        <v>224</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34"/>
@@ -2663,21 +2666,21 @@
       <c r="Z12" s="38"/>
     </row>
     <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="117" t="s">
-        <v>39</v>
+      <c r="A13" s="116" t="s">
+        <v>38</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D13" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G13" s="36" t="s">
         <v>23</v>
@@ -2703,24 +2706,24 @@
       <c r="Z13" s="13"/>
     </row>
     <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="117" t="s">
-        <v>39</v>
+      <c r="A14" s="116" t="s">
+        <v>38</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D14" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="G14" s="36" t="s">
         <v>26</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>27</v>
       </c>
       <c r="H14" s="37"/>
       <c r="I14" s="13"/>
@@ -2743,12 +2746,12 @@
       <c r="Z14" s="13"/>
     </row>
     <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="117" t="s">
-        <v>39</v>
+      <c r="A15" s="116" t="s">
+        <v>38</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D15" s="35" t="s">
         <v>2</v>
@@ -2760,7 +2763,7 @@
         <v>12</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" s="40"/>
       <c r="I15" s="13"/>
@@ -2783,18 +2786,18 @@
       <c r="Z15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="117" t="s">
-        <v>39</v>
+      <c r="A16" s="118" t="s">
+        <v>38</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D16" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F16" s="39"/>
       <c r="G16" s="36"/>
@@ -2820,7 +2823,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="106" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B17" s="41"/>
       <c r="C17" s="42"/>
@@ -2834,7 +2837,7 @@
       <c r="A18" s="45"/>
       <c r="B18" s="45"/>
       <c r="C18" s="107" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="45" t="s">
         <v>2</v>
@@ -2846,13 +2849,13 @@
         <v>12</v>
       </c>
       <c r="G18" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H18" s="45"/>
     </row>
     <row r="19" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="49"/>
       <c r="C19" s="50"/>
@@ -2860,10 +2863,10 @@
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
       <c r="G19" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="53" t="s">
         <v>43</v>
-      </c>
-      <c r="H19" s="53" t="s">
-        <v>44</v>
       </c>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
@@ -2887,7 +2890,7 @@
     <row r="20" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
       <c r="B20" s="103" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="51"/>
@@ -2895,7 +2898,7 @@
       <c r="F20" s="50"/>
       <c r="G20" s="52"/>
       <c r="H20" s="60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
@@ -2922,22 +2925,22 @@
         <v>1</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D21" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="114" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F21" s="61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G21" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="62" t="s">
         <v>47</v>
-      </c>
-      <c r="H21" s="62" t="s">
-        <v>48</v>
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
@@ -2960,11 +2963,11 @@
     </row>
     <row r="22" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="109" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="100"/>
       <c r="C22" s="108" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D22" s="51" t="s">
         <v>2</v>
@@ -3026,25 +3029,25 @@
         <v>2</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="96" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F24" s="96" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G24" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="13" t="s">
         <v>161</v>
-      </c>
-      <c r="H24" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
@@ -3066,11 +3069,11 @@
     </row>
     <row r="25" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="101"/>
       <c r="C25" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D25" s="64" t="s">
         <v>2</v>
@@ -3078,10 +3081,10 @@
       <c r="E25" s="61"/>
       <c r="F25" s="61"/>
       <c r="G25" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="66" t="s">
         <v>51</v>
-      </c>
-      <c r="H25" s="66" t="s">
-        <v>52</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -3106,7 +3109,7 @@
       <c r="A26" s="63"/>
       <c r="B26" s="100"/>
       <c r="C26" s="96" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D26" s="51" t="s">
         <v>2</v>
@@ -3118,10 +3121,10 @@
         <v>3</v>
       </c>
       <c r="G26" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="53" t="s">
         <v>59</v>
-      </c>
-      <c r="H26" s="53" t="s">
-        <v>60</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
@@ -3146,7 +3149,7 @@
       <c r="A27" s="63"/>
       <c r="B27" s="100"/>
       <c r="C27" s="96" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D27" s="51" t="s">
         <v>2</v>
@@ -3158,7 +3161,7 @@
         <v>1.5</v>
       </c>
       <c r="G27" s="52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H27" s="53"/>
       <c r="I27" s="13"/>
@@ -3182,7 +3185,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="104" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B28" s="100"/>
       <c r="C28" s="104"/>
@@ -3212,11 +3215,11 @@
     </row>
     <row r="29" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" s="100"/>
       <c r="C29" s="50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D29" s="51" t="s">
         <v>2</v>
@@ -3228,10 +3231,10 @@
         <v>75</v>
       </c>
       <c r="G29" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" s="53" t="s">
         <v>64</v>
-      </c>
-      <c r="H29" s="53" t="s">
-        <v>65</v>
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
@@ -3254,11 +3257,11 @@
     </row>
     <row r="30" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="100"/>
       <c r="C30" s="50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D30" s="51" t="s">
         <v>2</v>
@@ -3270,10 +3273,10 @@
         <v>450</v>
       </c>
       <c r="G30" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H30" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
@@ -3296,11 +3299,11 @@
     </row>
     <row r="31" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="100"/>
       <c r="C31" s="50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D31" s="51" t="s">
         <v>2</v>
@@ -3312,10 +3315,10 @@
         <v>3600</v>
       </c>
       <c r="G31" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H31" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
@@ -3370,19 +3373,19 @@
         <v>3</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D33" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E33" s="96" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F33" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="G33" s="52" t="s">
         <v>71</v>
-      </c>
-      <c r="G33" s="52" t="s">
-        <v>72</v>
       </c>
       <c r="H33" s="53"/>
       <c r="I33" s="13"/>
@@ -3406,24 +3409,24 @@
     </row>
     <row r="34" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="101"/>
       <c r="C34" s="108" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D34" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E34" s="61"/>
       <c r="F34" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G34" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="66" t="s">
         <v>51</v>
-      </c>
-      <c r="H34" s="66" t="s">
-        <v>52</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
@@ -3448,7 +3451,7 @@
       <c r="A35" s="63"/>
       <c r="B35" s="100"/>
       <c r="C35" s="50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D35" s="51" t="s">
         <v>2</v>
@@ -3460,7 +3463,7 @@
         <v>6</v>
       </c>
       <c r="G35" s="52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H35" s="53"/>
       <c r="I35" s="13"/>
@@ -3486,7 +3489,7 @@
       <c r="A36" s="63"/>
       <c r="B36" s="100"/>
       <c r="C36" s="50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D36" s="51" t="s">
         <v>2</v>
@@ -3520,7 +3523,7 @@
       <c r="A37" s="63"/>
       <c r="B37" s="100"/>
       <c r="C37" s="50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D37" s="51" t="s">
         <v>2</v>
@@ -3552,7 +3555,7 @@
     </row>
     <row r="38" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="104" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B38" s="100"/>
       <c r="C38" s="50"/>
@@ -3582,11 +3585,11 @@
     </row>
     <row r="39" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="100"/>
       <c r="C39" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D39" s="51" t="s">
         <v>2</v>
@@ -3598,10 +3601,10 @@
         <v>75</v>
       </c>
       <c r="G39" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="H39" s="53" t="s">
         <v>64</v>
-      </c>
-      <c r="H39" s="53" t="s">
-        <v>65</v>
       </c>
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
@@ -3624,11 +3627,11 @@
     </row>
     <row r="40" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="100"/>
       <c r="C40" s="50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D40" s="51" t="s">
         <v>2</v>
@@ -3640,10 +3643,10 @@
         <v>450</v>
       </c>
       <c r="G40" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H40" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
@@ -3666,11 +3669,11 @@
     </row>
     <row r="41" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="100"/>
       <c r="C41" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D41" s="51" t="s">
         <v>2</v>
@@ -3682,10 +3685,10 @@
         <v>3600</v>
       </c>
       <c r="G41" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H41" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
@@ -3736,23 +3739,23 @@
     </row>
     <row r="43" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" s="100">
         <v>4</v>
       </c>
       <c r="C43" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D43" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E43" s="50"/>
       <c r="F43" s="50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G43" s="52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H43" s="56"/>
       <c r="I43" s="13"/>
@@ -3776,24 +3779,24 @@
     </row>
     <row r="44" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="101"/>
       <c r="C44" s="108" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D44" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E44" s="61"/>
       <c r="F44" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G44" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H44" s="66" t="s">
         <v>51</v>
-      </c>
-      <c r="H44" s="66" t="s">
-        <v>52</v>
       </c>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
@@ -3816,11 +3819,11 @@
     </row>
     <row r="45" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="100"/>
       <c r="C45" s="50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D45" s="51" t="s">
         <v>2</v>
@@ -3830,7 +3833,7 @@
         <v>2</v>
       </c>
       <c r="G45" s="52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H45" s="53"/>
       <c r="I45" s="13"/>
@@ -3854,11 +3857,11 @@
     </row>
     <row r="46" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="100"/>
       <c r="C46" s="50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D46" s="51" t="s">
         <v>2</v>
@@ -3868,7 +3871,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H46" s="53"/>
       <c r="I46" s="13"/>
@@ -3892,11 +3895,11 @@
     </row>
     <row r="47" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="100"/>
       <c r="C47" s="50" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D47" s="51" t="s">
         <v>2</v>
@@ -3908,10 +3911,10 @@
         <v>75</v>
       </c>
       <c r="G47" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="H47" s="53" t="s">
         <v>64</v>
-      </c>
-      <c r="H47" s="53" t="s">
-        <v>65</v>
       </c>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
@@ -3934,11 +3937,11 @@
     </row>
     <row r="48" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="100"/>
       <c r="C48" s="50" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D48" s="51" t="s">
         <v>2</v>
@@ -3950,10 +3953,10 @@
         <v>450</v>
       </c>
       <c r="G48" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H48" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
@@ -3976,11 +3979,11 @@
     </row>
     <row r="49" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B49" s="100"/>
       <c r="C49" s="50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D49" s="51" t="s">
         <v>2</v>
@@ -3992,10 +3995,10 @@
         <v>3600</v>
       </c>
       <c r="G49" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H49" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
@@ -4046,23 +4049,23 @@
     </row>
     <row r="51" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B51" s="100">
         <v>5</v>
       </c>
       <c r="C51" s="50" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D51" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E51" s="50"/>
       <c r="F51" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G51" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H51" s="53"/>
       <c r="I51" s="13"/>
@@ -4086,24 +4089,24 @@
     </row>
     <row r="52" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B52" s="101"/>
       <c r="C52" s="61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D52" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E52" s="61"/>
       <c r="F52" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G52" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H52" s="66" t="s">
         <v>51</v>
-      </c>
-      <c r="H52" s="66" t="s">
-        <v>52</v>
       </c>
       <c r="I52" s="13"/>
       <c r="J52" s="13"/>
@@ -4126,11 +4129,11 @@
     </row>
     <row r="53" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B53" s="101"/>
       <c r="C53" s="50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D53" s="51" t="s">
         <v>2</v>
@@ -4160,11 +4163,11 @@
     </row>
     <row r="54" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B54" s="101"/>
       <c r="C54" s="50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D54" s="51" t="s">
         <v>2</v>
@@ -4194,11 +4197,11 @@
     </row>
     <row r="55" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B55" s="101"/>
       <c r="C55" s="50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D55" s="51" t="s">
         <v>2</v>
@@ -4208,7 +4211,7 @@
         <v>4.5</v>
       </c>
       <c r="G55" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H55" s="56"/>
       <c r="I55" s="13"/>
@@ -4232,11 +4235,11 @@
     </row>
     <row r="56" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" s="101"/>
       <c r="C56" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D56" s="51" t="s">
         <v>2</v>
@@ -4248,10 +4251,10 @@
         <v>75</v>
       </c>
       <c r="G56" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="H56" s="53" t="s">
         <v>64</v>
-      </c>
-      <c r="H56" s="53" t="s">
-        <v>65</v>
       </c>
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
@@ -4274,11 +4277,11 @@
     </row>
     <row r="57" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57" s="101"/>
       <c r="C57" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D57" s="51" t="s">
         <v>2</v>
@@ -4290,10 +4293,10 @@
         <v>450</v>
       </c>
       <c r="G57" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H57" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
@@ -4316,11 +4319,11 @@
     </row>
     <row r="58" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B58" s="101"/>
       <c r="C58" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D58" s="51" t="s">
         <v>2</v>
@@ -4332,10 +4335,10 @@
         <v>3600</v>
       </c>
       <c r="G58" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H58" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
@@ -4386,23 +4389,23 @@
     </row>
     <row r="60" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B60" s="100">
         <v>6</v>
       </c>
       <c r="C60" s="50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D60" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E60" s="50"/>
       <c r="F60" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="G60" s="52" t="s">
         <v>101</v>
-      </c>
-      <c r="G60" s="52" t="s">
-        <v>102</v>
       </c>
       <c r="H60" s="53"/>
       <c r="I60" s="13"/>
@@ -4431,7 +4434,7 @@
       </c>
       <c r="B61" s="100"/>
       <c r="C61" s="50" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D61" s="51"/>
       <c r="E61" s="50"/>
@@ -4464,20 +4467,20 @@
       </c>
       <c r="B62" s="101"/>
       <c r="C62" s="61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D62" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E62" s="61"/>
       <c r="F62" s="61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G62" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H62" s="66" t="s">
         <v>51</v>
-      </c>
-      <c r="H62" s="66" t="s">
-        <v>52</v>
       </c>
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
@@ -4528,23 +4531,23 @@
     </row>
     <row r="64" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B64" s="100">
         <v>7</v>
       </c>
       <c r="C64" s="50" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D64" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E64" s="50"/>
       <c r="F64" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="G64" s="52" t="s">
         <v>101</v>
-      </c>
-      <c r="G64" s="52" t="s">
-        <v>102</v>
       </c>
       <c r="H64" s="53"/>
       <c r="I64" s="13"/>
@@ -4573,7 +4576,7 @@
       </c>
       <c r="B65" s="100"/>
       <c r="C65" s="50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D65" s="97" t="s">
         <v>2</v>
@@ -4631,13 +4634,13 @@
     </row>
     <row r="67" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B67" s="100">
         <v>8</v>
       </c>
       <c r="C67" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D67" s="97" t="s">
         <v>2</v>
@@ -4672,7 +4675,7 @@
       </c>
       <c r="B68" s="102"/>
       <c r="C68" s="69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D68" s="98" t="s">
         <v>2</v>
@@ -4702,7 +4705,7 @@
     </row>
     <row r="69" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="99" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B69" s="99"/>
       <c r="C69" s="74"/>
@@ -4734,7 +4737,7 @@
       <c r="A70" s="78"/>
       <c r="B70" s="78"/>
       <c r="C70" s="74" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D70" s="75" t="s">
         <v>2</v>
@@ -4746,7 +4749,7 @@
         <v>750</v>
       </c>
       <c r="G70" s="76" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H70" s="77"/>
       <c r="I70" s="13"/>
@@ -4772,7 +4775,7 @@
       <c r="A71" s="78"/>
       <c r="B71" s="78"/>
       <c r="C71" s="74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D71" s="75" t="s">
         <v>2</v>
@@ -4784,7 +4787,7 @@
         <v>80</v>
       </c>
       <c r="G71" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H71" s="77"/>
       <c r="I71" s="13"/>
@@ -4810,7 +4813,7 @@
       <c r="A72" s="78"/>
       <c r="B72" s="78"/>
       <c r="C72" s="74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D72" s="75" t="s">
         <v>2</v>
@@ -4822,7 +4825,7 @@
         <v>900</v>
       </c>
       <c r="G72" s="76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H72" s="77"/>
       <c r="I72" s="13"/>
@@ -4848,7 +4851,7 @@
       <c r="A73" s="78"/>
       <c r="B73" s="78"/>
       <c r="C73" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D73" s="75" t="s">
         <v>2</v>
@@ -4860,7 +4863,7 @@
         <v>1200</v>
       </c>
       <c r="G73" s="76" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H73" s="77"/>
       <c r="I73" s="13"/>
@@ -4886,7 +4889,7 @@
       <c r="A74" s="78"/>
       <c r="B74" s="78"/>
       <c r="C74" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D74" s="75" t="s">
         <v>2</v>
@@ -4898,10 +4901,10 @@
         <v>105</v>
       </c>
       <c r="G74" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="H74" s="77" t="s">
         <v>117</v>
-      </c>
-      <c r="H74" s="77" t="s">
-        <v>118</v>
       </c>
       <c r="I74" s="13"/>
       <c r="J74" s="13"/>
@@ -4926,7 +4929,7 @@
       <c r="A75" s="78"/>
       <c r="B75" s="78"/>
       <c r="C75" s="74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D75" s="75" t="s">
         <v>2</v>
@@ -4938,10 +4941,10 @@
         <v>12600</v>
       </c>
       <c r="G75" s="76" t="s">
+        <v>119</v>
+      </c>
+      <c r="H75" s="77" t="s">
         <v>120</v>
-      </c>
-      <c r="H75" s="77" t="s">
-        <v>121</v>
       </c>
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
@@ -4966,7 +4969,7 @@
       <c r="A76" s="78"/>
       <c r="B76" s="78"/>
       <c r="C76" s="74" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D76" s="75" t="s">
         <v>2</v>
@@ -4978,10 +4981,10 @@
         <v>3</v>
       </c>
       <c r="G76" s="76" t="s">
+        <v>122</v>
+      </c>
+      <c r="H76" s="77" t="s">
         <v>123</v>
-      </c>
-      <c r="H76" s="77" t="s">
-        <v>124</v>
       </c>
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
@@ -5004,24 +5007,24 @@
     </row>
     <row r="77" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B77" s="79"/>
       <c r="C77" s="80" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D77" s="81" t="s">
         <v>2</v>
       </c>
       <c r="E77" s="111" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F77" s="80"/>
       <c r="G77" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="H77" s="83" t="s">
         <v>126</v>
-      </c>
-      <c r="H77" s="83" t="s">
-        <v>127</v>
       </c>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
@@ -5044,7 +5047,7 @@
     </row>
     <row r="78" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="99" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B78" s="99"/>
       <c r="C78" s="74"/>
@@ -5076,7 +5079,7 @@
       <c r="A79" s="78"/>
       <c r="B79" s="78"/>
       <c r="C79" s="112" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D79" s="75" t="s">
         <v>2</v>
@@ -5088,10 +5091,10 @@
         <v>45</v>
       </c>
       <c r="G79" s="113" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H79" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I79" s="13"/>
       <c r="J79" s="13"/>
@@ -5116,7 +5119,7 @@
       <c r="A80" s="78"/>
       <c r="B80" s="78"/>
       <c r="C80" s="74" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D80" s="75" t="s">
         <v>2</v>
@@ -5128,10 +5131,10 @@
         <v>75</v>
       </c>
       <c r="G80" s="76" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H80" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I80" s="13"/>
       <c r="J80" s="13"/>
@@ -5156,7 +5159,7 @@
       <c r="A81" s="78"/>
       <c r="B81" s="78"/>
       <c r="C81" s="74" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D81" s="75" t="s">
         <v>2</v>
@@ -5168,10 +5171,10 @@
         <v>450</v>
       </c>
       <c r="G81" s="76" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H81" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I81" s="13"/>
       <c r="J81" s="13"/>
@@ -5196,7 +5199,7 @@
       <c r="A82" s="79"/>
       <c r="B82" s="79"/>
       <c r="C82" s="80" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D82" s="81" t="s">
         <v>2</v>
@@ -5208,10 +5211,10 @@
         <v>3600</v>
       </c>
       <c r="G82" s="82" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H82" s="83" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
@@ -14442,7 +14445,7 @@
   <dimension ref="A1:T500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14456,37 +14459,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="89" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C1" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="89" t="s">
         <v>226</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="E1" s="89" t="s">
         <v>227</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="F1" s="89" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" s="89" t="s">
         <v>228</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="H1" s="89" t="s">
         <v>229</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="I1" s="89" t="s">
         <v>230</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="J1" s="90" t="s">
         <v>231</v>
       </c>
-      <c r="I1" s="89" t="s">
+      <c r="K1" s="90" t="s">
         <v>232</v>
-      </c>
-      <c r="J1" s="90" t="s">
-        <v>233</v>
-      </c>
-      <c r="K1" s="90" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
@@ -14495,7 +14498,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="91" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C2" s="90">
         <v>150</v>
@@ -14532,7 +14535,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C3" s="90">
         <v>150</v>
@@ -14569,7 +14572,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="91" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C4" s="90">
         <v>150</v>
@@ -16040,7 +16043,7 @@
   <dimension ref="A1:K98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16052,37 +16055,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="89" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="89" t="s">
-        <v>235</v>
-      </c>
-      <c r="C1" s="89" t="s">
+      <c r="D1" s="89" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="E1" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="F1" s="89" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="G1" s="89" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="H1" s="89" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="I1" s="89" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="89" t="s">
-        <v>144</v>
-      </c>
       <c r="J1" s="89" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K1" s="90" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -20556,8 +20559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W998"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20901,7 +20904,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>2</v>
@@ -20938,7 +20941,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C12" s="35" t="s">
         <v>2</v>
@@ -20973,14 +20976,14 @@
         <v>#</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="34" t="str">
         <f>'User Interface'!E13</f>
-        <v>[[3,1]]</v>
+        <v>[[2,3,1,]]</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>22</v>
@@ -21010,14 +21013,14 @@
         <v>#</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="34" t="str">
         <f>'User Interface'!E14</f>
-        <v>[[500,500]]</v>
+        <v>[[215, 215]]</v>
       </c>
       <c r="E14" s="34" t="s">
         <v>22</v>
@@ -21047,7 +21050,7 @@
         <v>#</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>2</v>
@@ -21084,7 +21087,7 @@
         <v>#</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>2</v>
@@ -21115,7 +21118,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
@@ -21125,7 +21128,7 @@
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="45"/>
       <c r="B18" s="45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="45"/>
       <c r="D18" s="34">
@@ -21138,7 +21141,7 @@
     </row>
     <row r="19" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="50"/>
       <c r="C19" s="51"/>
@@ -21190,10 +21193,10 @@
     </row>
     <row r="21" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="55" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" s="55" t="s">
-        <v>40</v>
       </c>
       <c r="C21" s="51" t="s">
         <v>2</v>
@@ -21225,10 +21228,10 @@
     </row>
     <row r="22" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="51" t="s">
         <v>2</v>
@@ -21285,7 +21288,7 @@
     </row>
     <row r="24" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="50"/>
       <c r="C24" s="51"/>
@@ -21341,7 +21344,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="51" t="s">
         <v>2</v>
@@ -21378,13 +21381,13 @@
         <v>#</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="61" t="s">
         <v>15</v>
@@ -21439,7 +21442,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="51" t="s">
         <v>2</v>
@@ -21476,7 +21479,7 @@
         <v>#</v>
       </c>
       <c r="B30" s="61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="64" t="s">
         <v>2</v>
@@ -21513,7 +21516,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="51" t="s">
         <v>2</v>
@@ -21550,7 +21553,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="51" t="s">
         <v>2</v>
@@ -21587,7 +21590,7 @@
         <v>#</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="51" t="s">
         <v>2</v>
@@ -21624,7 +21627,7 @@
         <v>#</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="51" t="s">
         <v>2</v>
@@ -21661,7 +21664,7 @@
         <v>#</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="51" t="s">
         <v>2</v>
@@ -21723,7 +21726,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>2</v>
@@ -21760,7 +21763,7 @@
         <v>#</v>
       </c>
       <c r="B38" s="61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="64" t="s">
         <v>2</v>
@@ -21797,7 +21800,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>2</v>
@@ -21834,7 +21837,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="108" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C40" s="51" t="s">
         <v>2</v>
@@ -21869,7 +21872,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="108" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C41" s="51" t="s">
         <v>2</v>
@@ -21904,7 +21907,7 @@
         <v>#</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="51" t="s">
         <v>2</v>
@@ -21941,7 +21944,7 @@
         <v>#</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" s="51" t="s">
         <v>2</v>
@@ -21978,7 +21981,7 @@
         <v>#</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="51" t="s">
         <v>2</v>
@@ -22036,16 +22039,16 @@
     </row>
     <row r="46" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E46" s="50" t="s">
         <v>22</v>
@@ -22071,16 +22074,16 @@
     </row>
     <row r="47" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E47" s="61" t="s">
         <v>15</v>
@@ -22106,10 +22109,10 @@
     </row>
     <row r="48" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="51" t="s">
         <v>2</v>
@@ -22141,10 +22144,10 @@
     </row>
     <row r="49" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B49" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="51" t="s">
         <v>2</v>
@@ -22176,10 +22179,10 @@
     </row>
     <row r="50" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="51" t="s">
         <v>2</v>
@@ -22211,10 +22214,10 @@
     </row>
     <row r="51" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" s="51" t="s">
         <v>2</v>
@@ -22246,10 +22249,10 @@
     </row>
     <row r="52" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C52" s="51" t="s">
         <v>2</v>
@@ -22306,16 +22309,16 @@
     </row>
     <row r="54" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C54" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E54" s="50" t="s">
         <v>22</v>
@@ -22341,16 +22344,16 @@
     </row>
     <row r="55" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B55" s="61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C55" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D55" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E55" s="61" t="s">
         <v>15</v>
@@ -22376,10 +22379,10 @@
     </row>
     <row r="56" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" s="67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C56" s="51" t="s">
         <v>2</v>
@@ -22411,10 +22414,10 @@
     </row>
     <row r="57" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C57" s="51" t="s">
         <v>2</v>
@@ -22446,10 +22449,10 @@
     </row>
     <row r="58" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B58" s="50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C58" s="51" t="s">
         <v>2</v>
@@ -22481,10 +22484,10 @@
     </row>
     <row r="59" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B59" s="50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C59" s="51" t="s">
         <v>2</v>
@@ -22541,16 +22544,16 @@
     </row>
     <row r="61" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C61" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D61" s="50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E61" s="50" t="s">
         <v>22</v>
@@ -22576,16 +22579,16 @@
     </row>
     <row r="62" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62" s="61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C62" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E62" s="61" t="s">
         <v>15</v>
@@ -22636,16 +22639,16 @@
     </row>
     <row r="64" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B64" s="50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C64" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D64" s="50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E64" s="50" t="s">
         <v>22</v>
@@ -22671,16 +22674,16 @@
     </row>
     <row r="65" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="68" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B65" s="69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C65" s="70" t="s">
         <v>2</v>
       </c>
       <c r="D65" s="69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E65" s="69" t="s">
         <v>15</v>
@@ -22706,7 +22709,7 @@
     </row>
     <row r="66" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B66" s="74"/>
       <c r="C66" s="75"/>
@@ -22734,7 +22737,7 @@
     <row r="67" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="78"/>
       <c r="B67" s="74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C67" s="75" t="s">
         <v>2</v>
@@ -22768,7 +22771,7 @@
     <row r="68" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="78"/>
       <c r="B68" s="74" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C68" s="75" t="s">
         <v>2</v>
@@ -22802,7 +22805,7 @@
     <row r="69" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="78"/>
       <c r="B69" s="74" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C69" s="75" t="s">
         <v>2</v>
@@ -22836,7 +22839,7 @@
     <row r="70" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="78"/>
       <c r="B70" s="74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C70" s="75" t="s">
         <v>2</v>
@@ -22870,7 +22873,7 @@
     <row r="71" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="78"/>
       <c r="B71" s="74" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C71" s="75" t="s">
         <v>2</v>
@@ -22904,7 +22907,7 @@
     <row r="72" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="78"/>
       <c r="B72" s="74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C72" s="75" t="s">
         <v>2</v>
@@ -22938,7 +22941,7 @@
     <row r="73" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="78"/>
       <c r="B73" s="74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C73" s="75" t="s">
         <v>2</v>
@@ -22972,7 +22975,7 @@
     <row r="74" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="79"/>
       <c r="B74" s="80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C74" s="81" t="s">
         <v>2</v>
@@ -23005,7 +23008,7 @@
     </row>
     <row r="75" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B75" s="74"/>
       <c r="C75" s="75"/>
@@ -23033,7 +23036,7 @@
     <row r="76" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="78"/>
       <c r="B76" s="74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C76" s="75" t="s">
         <v>2</v>
@@ -23067,7 +23070,7 @@
     <row r="77" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="78"/>
       <c r="B77" s="74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C77" s="75" t="s">
         <v>2</v>
@@ -23101,7 +23104,7 @@
     <row r="78" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="78"/>
       <c r="B78" s="74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C78" s="75" t="s">
         <v>2</v>
@@ -23135,7 +23138,7 @@
     <row r="79" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="79"/>
       <c r="B79" s="80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C79" s="81" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Revert "refact gettsheettarget into smaller funcitons:"
This reverts commit bd8e39e48987929eac0cb7997e010667ca44ee4f.
</commit_message>
<xml_diff>
--- a/MIT_PVLab_Template.xlsx
+++ b/MIT_PVLab_Template.xlsx
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>exp1_vols</t>
+  </si>
+  <si>
+    <t>[[500,500]]</t>
   </si>
   <si>
     <t xml:space="preserve">Min and Max volumes for each portion of the experiment. </t>
@@ -1172,6 +1175,9 @@
     <t>Precursor3 (ul)</t>
   </si>
   <si>
+    <t>Precurso4 (ul)</t>
+  </si>
+  <si>
     <t>Precursor5 (ul)</t>
   </si>
   <si>
@@ -1220,13 +1226,7 @@
     <t>exp2_name</t>
   </si>
   <si>
-    <t>Precursor4 (ul)</t>
-  </si>
-  <si>
-    <t>[[2,3,1,]]</t>
-  </si>
-  <si>
-    <t>[[215, 215]]</t>
+    <t>[[3,1]]</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1820,9 +1820,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2215,8 +2212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2309,7 +2306,7 @@
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="92" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D3" s="93" t="s">
         <v>2</v>
@@ -2321,7 +2318,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="13"/>
@@ -2353,16 +2350,16 @@
         <v>2</v>
       </c>
       <c r="E4" s="94" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -2417,7 +2414,7 @@
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>2</v>
@@ -2451,7 +2448,7 @@
     </row>
     <row r="7" spans="1:26" s="32" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="105" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="27"/>
@@ -2485,16 +2482,16 @@
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="34" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D8" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G8" s="36" t="s">
         <v>23</v>
@@ -2525,22 +2522,22 @@
       <c r="A9" s="33"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D9" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
@@ -2565,7 +2562,7 @@
       <c r="A10" s="33"/>
       <c r="B10" s="33"/>
       <c r="C10" s="34" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D10" s="35" t="s">
         <v>2</v>
@@ -2577,10 +2574,10 @@
         <v>12</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
@@ -2605,13 +2602,13 @@
       <c r="A11" s="33"/>
       <c r="B11" s="33"/>
       <c r="C11" s="34" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D11" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="36"/>
@@ -2636,8 +2633,8 @@
       <c r="Z11" s="38"/>
     </row>
     <row r="12" spans="1:26" s="32" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="117" t="s">
-        <v>224</v>
+      <c r="A12" s="116" t="s">
+        <v>225</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34"/>
@@ -2666,21 +2663,21 @@
       <c r="Z12" s="38"/>
     </row>
     <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="116" t="s">
-        <v>38</v>
+      <c r="A13" s="117" t="s">
+        <v>39</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D13" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G13" s="36" t="s">
         <v>23</v>
@@ -2706,24 +2703,24 @@
       <c r="Z13" s="13"/>
     </row>
     <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="116" t="s">
-        <v>38</v>
+      <c r="A14" s="117" t="s">
+        <v>39</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D14" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>246</v>
+        <v>26</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G14" s="36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H14" s="37"/>
       <c r="I14" s="13"/>
@@ -2746,12 +2743,12 @@
       <c r="Z14" s="13"/>
     </row>
     <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="116" t="s">
-        <v>38</v>
+      <c r="A15" s="117" t="s">
+        <v>39</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D15" s="35" t="s">
         <v>2</v>
@@ -2763,7 +2760,7 @@
         <v>12</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H15" s="40"/>
       <c r="I15" s="13"/>
@@ -2786,18 +2783,18 @@
       <c r="Z15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="118" t="s">
-        <v>38</v>
+      <c r="A16" s="117" t="s">
+        <v>39</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D16" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F16" s="39"/>
       <c r="G16" s="36"/>
@@ -2823,7 +2820,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="106" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B17" s="41"/>
       <c r="C17" s="42"/>
@@ -2837,7 +2834,7 @@
       <c r="A18" s="45"/>
       <c r="B18" s="45"/>
       <c r="C18" s="107" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="45" t="s">
         <v>2</v>
@@ -2849,13 +2846,13 @@
         <v>12</v>
       </c>
       <c r="G18" s="48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H18" s="45"/>
     </row>
     <row r="19" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="49"/>
       <c r="C19" s="50"/>
@@ -2863,10 +2860,10 @@
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
       <c r="G19" s="52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H19" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
@@ -2890,7 +2887,7 @@
     <row r="20" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
       <c r="B20" s="103" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="51"/>
@@ -2898,7 +2895,7 @@
       <c r="F20" s="50"/>
       <c r="G20" s="52"/>
       <c r="H20" s="60" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
@@ -2925,22 +2922,22 @@
         <v>1</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D21" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="114" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F21" s="61" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G21" s="52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H21" s="62" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
@@ -2963,11 +2960,11 @@
     </row>
     <row r="22" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="109" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="100"/>
       <c r="C22" s="108" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D22" s="51" t="s">
         <v>2</v>
@@ -3029,25 +3026,25 @@
         <v>2</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D24" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="96" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F24" s="96" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G24" s="52" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H24" s="56" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
@@ -3069,11 +3066,11 @@
     </row>
     <row r="25" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="101"/>
       <c r="C25" s="50" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D25" s="64" t="s">
         <v>2</v>
@@ -3081,10 +3078,10 @@
       <c r="E25" s="61"/>
       <c r="F25" s="61"/>
       <c r="G25" s="65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H25" s="66" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -3109,7 +3106,7 @@
       <c r="A26" s="63"/>
       <c r="B26" s="100"/>
       <c r="C26" s="96" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D26" s="51" t="s">
         <v>2</v>
@@ -3121,10 +3118,10 @@
         <v>3</v>
       </c>
       <c r="G26" s="52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H26" s="53" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
@@ -3149,7 +3146,7 @@
       <c r="A27" s="63"/>
       <c r="B27" s="100"/>
       <c r="C27" s="96" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D27" s="51" t="s">
         <v>2</v>
@@ -3161,7 +3158,7 @@
         <v>1.5</v>
       </c>
       <c r="G27" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H27" s="53"/>
       <c r="I27" s="13"/>
@@ -3185,7 +3182,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="104" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B28" s="100"/>
       <c r="C28" s="104"/>
@@ -3215,11 +3212,11 @@
     </row>
     <row r="29" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B29" s="100"/>
       <c r="C29" s="50" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D29" s="51" t="s">
         <v>2</v>
@@ -3231,10 +3228,10 @@
         <v>75</v>
       </c>
       <c r="G29" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H29" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
@@ -3257,11 +3254,11 @@
     </row>
     <row r="30" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B30" s="100"/>
       <c r="C30" s="50" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D30" s="51" t="s">
         <v>2</v>
@@ -3273,10 +3270,10 @@
         <v>450</v>
       </c>
       <c r="G30" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H30" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
@@ -3299,11 +3296,11 @@
     </row>
     <row r="31" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" s="100"/>
       <c r="C31" s="50" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D31" s="51" t="s">
         <v>2</v>
@@ -3315,10 +3312,10 @@
         <v>3600</v>
       </c>
       <c r="G31" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H31" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
@@ -3373,19 +3370,19 @@
         <v>3</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D33" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E33" s="96" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F33" s="50" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G33" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H33" s="53"/>
       <c r="I33" s="13"/>
@@ -3409,24 +3406,24 @@
     </row>
     <row r="34" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34" s="101"/>
       <c r="C34" s="108" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D34" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E34" s="61"/>
       <c r="F34" s="61" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G34" s="65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H34" s="66" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
@@ -3451,7 +3448,7 @@
       <c r="A35" s="63"/>
       <c r="B35" s="100"/>
       <c r="C35" s="50" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D35" s="51" t="s">
         <v>2</v>
@@ -3463,7 +3460,7 @@
         <v>6</v>
       </c>
       <c r="G35" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H35" s="53"/>
       <c r="I35" s="13"/>
@@ -3489,7 +3486,7 @@
       <c r="A36" s="63"/>
       <c r="B36" s="100"/>
       <c r="C36" s="50" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D36" s="51" t="s">
         <v>2</v>
@@ -3523,7 +3520,7 @@
       <c r="A37" s="63"/>
       <c r="B37" s="100"/>
       <c r="C37" s="50" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D37" s="51" t="s">
         <v>2</v>
@@ -3555,7 +3552,7 @@
     </row>
     <row r="38" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="104" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B38" s="100"/>
       <c r="C38" s="50"/>
@@ -3585,11 +3582,11 @@
     </row>
     <row r="39" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="100"/>
       <c r="C39" s="50" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D39" s="51" t="s">
         <v>2</v>
@@ -3601,10 +3598,10 @@
         <v>75</v>
       </c>
       <c r="G39" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H39" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
@@ -3627,11 +3624,11 @@
     </row>
     <row r="40" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="100"/>
       <c r="C40" s="50" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D40" s="51" t="s">
         <v>2</v>
@@ -3643,10 +3640,10 @@
         <v>450</v>
       </c>
       <c r="G40" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H40" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
@@ -3669,11 +3666,11 @@
     </row>
     <row r="41" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" s="100"/>
       <c r="C41" s="50" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D41" s="51" t="s">
         <v>2</v>
@@ -3685,10 +3682,10 @@
         <v>3600</v>
       </c>
       <c r="G41" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H41" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
@@ -3739,23 +3736,23 @@
     </row>
     <row r="43" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B43" s="100">
         <v>4</v>
       </c>
       <c r="C43" s="50" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D43" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E43" s="50"/>
       <c r="F43" s="50" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G43" s="52" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H43" s="56"/>
       <c r="I43" s="13"/>
@@ -3779,24 +3776,24 @@
     </row>
     <row r="44" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B44" s="101"/>
       <c r="C44" s="108" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D44" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E44" s="61"/>
       <c r="F44" s="61" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G44" s="65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H44" s="66" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
@@ -3819,11 +3816,11 @@
     </row>
     <row r="45" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B45" s="100"/>
       <c r="C45" s="50" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D45" s="51" t="s">
         <v>2</v>
@@ -3833,7 +3830,7 @@
         <v>2</v>
       </c>
       <c r="G45" s="52" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H45" s="53"/>
       <c r="I45" s="13"/>
@@ -3857,11 +3854,11 @@
     </row>
     <row r="46" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B46" s="100"/>
       <c r="C46" s="50" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D46" s="51" t="s">
         <v>2</v>
@@ -3871,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="52" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H46" s="53"/>
       <c r="I46" s="13"/>
@@ -3895,11 +3892,11 @@
     </row>
     <row r="47" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B47" s="100"/>
       <c r="C47" s="50" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D47" s="51" t="s">
         <v>2</v>
@@ -3911,10 +3908,10 @@
         <v>75</v>
       </c>
       <c r="G47" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H47" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
@@ -3937,11 +3934,11 @@
     </row>
     <row r="48" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B48" s="100"/>
       <c r="C48" s="50" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D48" s="51" t="s">
         <v>2</v>
@@ -3953,10 +3950,10 @@
         <v>450</v>
       </c>
       <c r="G48" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H48" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
@@ -3979,11 +3976,11 @@
     </row>
     <row r="49" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B49" s="100"/>
       <c r="C49" s="50" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D49" s="51" t="s">
         <v>2</v>
@@ -3995,10 +3992,10 @@
         <v>3600</v>
       </c>
       <c r="G49" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H49" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
@@ -4049,23 +4046,23 @@
     </row>
     <row r="51" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B51" s="100">
         <v>5</v>
       </c>
       <c r="C51" s="50" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D51" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E51" s="50"/>
       <c r="F51" s="50" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G51" s="52" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H51" s="53"/>
       <c r="I51" s="13"/>
@@ -4089,24 +4086,24 @@
     </row>
     <row r="52" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B52" s="101"/>
       <c r="C52" s="61" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D52" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E52" s="61"/>
       <c r="F52" s="61" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G52" s="65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H52" s="66" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I52" s="13"/>
       <c r="J52" s="13"/>
@@ -4129,11 +4126,11 @@
     </row>
     <row r="53" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B53" s="101"/>
       <c r="C53" s="50" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D53" s="51" t="s">
         <v>2</v>
@@ -4163,11 +4160,11 @@
     </row>
     <row r="54" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B54" s="101"/>
       <c r="C54" s="50" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D54" s="51" t="s">
         <v>2</v>
@@ -4197,11 +4194,11 @@
     </row>
     <row r="55" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B55" s="101"/>
       <c r="C55" s="50" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D55" s="51" t="s">
         <v>2</v>
@@ -4211,7 +4208,7 @@
         <v>4.5</v>
       </c>
       <c r="G55" s="52" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H55" s="56"/>
       <c r="I55" s="13"/>
@@ -4235,11 +4232,11 @@
     </row>
     <row r="56" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B56" s="101"/>
       <c r="C56" s="50" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D56" s="51" t="s">
         <v>2</v>
@@ -4251,10 +4248,10 @@
         <v>75</v>
       </c>
       <c r="G56" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H56" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
@@ -4277,11 +4274,11 @@
     </row>
     <row r="57" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B57" s="101"/>
       <c r="C57" s="50" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D57" s="51" t="s">
         <v>2</v>
@@ -4293,10 +4290,10 @@
         <v>450</v>
       </c>
       <c r="G57" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H57" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
@@ -4319,11 +4316,11 @@
     </row>
     <row r="58" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B58" s="101"/>
       <c r="C58" s="50" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D58" s="51" t="s">
         <v>2</v>
@@ -4335,10 +4332,10 @@
         <v>3600</v>
       </c>
       <c r="G58" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H58" s="53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
@@ -4389,23 +4386,23 @@
     </row>
     <row r="60" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B60" s="100">
         <v>6</v>
       </c>
       <c r="C60" s="50" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D60" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E60" s="50"/>
       <c r="F60" s="50" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G60" s="52" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H60" s="53"/>
       <c r="I60" s="13"/>
@@ -4434,7 +4431,7 @@
       </c>
       <c r="B61" s="100"/>
       <c r="C61" s="50" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D61" s="51"/>
       <c r="E61" s="50"/>
@@ -4467,20 +4464,20 @@
       </c>
       <c r="B62" s="101"/>
       <c r="C62" s="61" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D62" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E62" s="61"/>
       <c r="F62" s="61" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G62" s="65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H62" s="66" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
@@ -4531,23 +4528,23 @@
     </row>
     <row r="64" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B64" s="100">
         <v>7</v>
       </c>
       <c r="C64" s="50" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D64" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E64" s="50"/>
       <c r="F64" s="50" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G64" s="52" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H64" s="53"/>
       <c r="I64" s="13"/>
@@ -4576,7 +4573,7 @@
       </c>
       <c r="B65" s="100"/>
       <c r="C65" s="50" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D65" s="97" t="s">
         <v>2</v>
@@ -4634,13 +4631,13 @@
     </row>
     <row r="67" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B67" s="100">
         <v>8</v>
       </c>
       <c r="C67" s="50" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D67" s="97" t="s">
         <v>2</v>
@@ -4675,7 +4672,7 @@
       </c>
       <c r="B68" s="102"/>
       <c r="C68" s="69" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D68" s="98" t="s">
         <v>2</v>
@@ -4705,7 +4702,7 @@
     </row>
     <row r="69" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="99" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B69" s="99"/>
       <c r="C69" s="74"/>
@@ -4737,7 +4734,7 @@
       <c r="A70" s="78"/>
       <c r="B70" s="78"/>
       <c r="C70" s="74" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D70" s="75" t="s">
         <v>2</v>
@@ -4749,7 +4746,7 @@
         <v>750</v>
       </c>
       <c r="G70" s="76" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H70" s="77"/>
       <c r="I70" s="13"/>
@@ -4775,7 +4772,7 @@
       <c r="A71" s="78"/>
       <c r="B71" s="78"/>
       <c r="C71" s="74" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D71" s="75" t="s">
         <v>2</v>
@@ -4787,7 +4784,7 @@
         <v>80</v>
       </c>
       <c r="G71" s="76" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H71" s="77"/>
       <c r="I71" s="13"/>
@@ -4813,7 +4810,7 @@
       <c r="A72" s="78"/>
       <c r="B72" s="78"/>
       <c r="C72" s="74" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D72" s="75" t="s">
         <v>2</v>
@@ -4825,7 +4822,7 @@
         <v>900</v>
       </c>
       <c r="G72" s="76" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H72" s="77"/>
       <c r="I72" s="13"/>
@@ -4851,7 +4848,7 @@
       <c r="A73" s="78"/>
       <c r="B73" s="78"/>
       <c r="C73" s="74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D73" s="75" t="s">
         <v>2</v>
@@ -4863,7 +4860,7 @@
         <v>1200</v>
       </c>
       <c r="G73" s="76" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H73" s="77"/>
       <c r="I73" s="13"/>
@@ -4889,7 +4886,7 @@
       <c r="A74" s="78"/>
       <c r="B74" s="78"/>
       <c r="C74" s="74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D74" s="75" t="s">
         <v>2</v>
@@ -4901,10 +4898,10 @@
         <v>105</v>
       </c>
       <c r="G74" s="76" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H74" s="77" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I74" s="13"/>
       <c r="J74" s="13"/>
@@ -4929,7 +4926,7 @@
       <c r="A75" s="78"/>
       <c r="B75" s="78"/>
       <c r="C75" s="74" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D75" s="75" t="s">
         <v>2</v>
@@ -4941,10 +4938,10 @@
         <v>12600</v>
       </c>
       <c r="G75" s="76" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H75" s="77" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
@@ -4969,7 +4966,7 @@
       <c r="A76" s="78"/>
       <c r="B76" s="78"/>
       <c r="C76" s="74" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D76" s="75" t="s">
         <v>2</v>
@@ -4981,10 +4978,10 @@
         <v>3</v>
       </c>
       <c r="G76" s="76" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H76" s="77" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
@@ -5007,24 +5004,24 @@
     </row>
     <row r="77" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="79" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B77" s="79"/>
       <c r="C77" s="80" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D77" s="81" t="s">
         <v>2</v>
       </c>
       <c r="E77" s="111" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F77" s="80"/>
       <c r="G77" s="82" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H77" s="83" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
@@ -5047,7 +5044,7 @@
     </row>
     <row r="78" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="99" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B78" s="99"/>
       <c r="C78" s="74"/>
@@ -5079,7 +5076,7 @@
       <c r="A79" s="78"/>
       <c r="B79" s="78"/>
       <c r="C79" s="112" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D79" s="75" t="s">
         <v>2</v>
@@ -5091,10 +5088,10 @@
         <v>45</v>
       </c>
       <c r="G79" s="113" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H79" s="77" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I79" s="13"/>
       <c r="J79" s="13"/>
@@ -5119,7 +5116,7 @@
       <c r="A80" s="78"/>
       <c r="B80" s="78"/>
       <c r="C80" s="74" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D80" s="75" t="s">
         <v>2</v>
@@ -5131,10 +5128,10 @@
         <v>75</v>
       </c>
       <c r="G80" s="76" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H80" s="77" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I80" s="13"/>
       <c r="J80" s="13"/>
@@ -5159,7 +5156,7 @@
       <c r="A81" s="78"/>
       <c r="B81" s="78"/>
       <c r="C81" s="74" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D81" s="75" t="s">
         <v>2</v>
@@ -5171,10 +5168,10 @@
         <v>450</v>
       </c>
       <c r="G81" s="76" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H81" s="77" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I81" s="13"/>
       <c r="J81" s="13"/>
@@ -5199,7 +5196,7 @@
       <c r="A82" s="79"/>
       <c r="B82" s="79"/>
       <c r="C82" s="80" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D82" s="81" t="s">
         <v>2</v>
@@ -5211,10 +5208,10 @@
         <v>3600</v>
       </c>
       <c r="G82" s="82" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H82" s="83" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
@@ -14445,7 +14442,7 @@
   <dimension ref="A1:T500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14459,37 +14456,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B1" s="89" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="89" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" s="89" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="89" t="s">
+        <v>229</v>
+      </c>
+      <c r="G1" s="89" t="s">
+        <v>230</v>
+      </c>
+      <c r="H1" s="89" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1" s="89" t="s">
+        <v>232</v>
+      </c>
+      <c r="J1" s="90" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="89" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="89" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="89" t="s">
-        <v>227</v>
-      </c>
-      <c r="F1" s="89" t="s">
-        <v>244</v>
-      </c>
-      <c r="G1" s="89" t="s">
-        <v>228</v>
-      </c>
-      <c r="H1" s="89" t="s">
-        <v>229</v>
-      </c>
-      <c r="I1" s="89" t="s">
-        <v>230</v>
-      </c>
-      <c r="J1" s="90" t="s">
-        <v>231</v>
-      </c>
       <c r="K1" s="90" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
@@ -14498,7 +14495,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="91" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C2" s="90">
         <v>150</v>
@@ -14535,7 +14532,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C3" s="90">
         <v>150</v>
@@ -14572,7 +14569,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="91" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C4" s="90">
         <v>150</v>
@@ -16043,7 +16040,7 @@
   <dimension ref="A1:K98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16055,37 +16052,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B1" s="89" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C1" s="89" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D1" s="89" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E1" s="89" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F1" s="89" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G1" s="89" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H1" s="89" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I1" s="89" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J1" s="89" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="K1" s="90" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -20559,8 +20556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20904,7 +20901,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>2</v>
@@ -20941,7 +20938,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C12" s="35" t="s">
         <v>2</v>
@@ -20976,14 +20973,14 @@
         <v>#</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="34" t="str">
         <f>'User Interface'!E13</f>
-        <v>[[2,3,1,]]</v>
+        <v>[[3,1]]</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>22</v>
@@ -21013,14 +21010,14 @@
         <v>#</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="34" t="str">
         <f>'User Interface'!E14</f>
-        <v>[[215, 215]]</v>
+        <v>[[500,500]]</v>
       </c>
       <c r="E14" s="34" t="s">
         <v>22</v>
@@ -21050,7 +21047,7 @@
         <v>#</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>2</v>
@@ -21087,7 +21084,7 @@
         <v>#</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>2</v>
@@ -21118,7 +21115,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="41" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
@@ -21128,7 +21125,7 @@
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="45"/>
       <c r="B18" s="45" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C18" s="45"/>
       <c r="D18" s="34">
@@ -21141,7 +21138,7 @@
     </row>
     <row r="19" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" s="50"/>
       <c r="C19" s="51"/>
@@ -21193,10 +21190,10 @@
     </row>
     <row r="21" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B21" s="55" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" s="51" t="s">
         <v>2</v>
@@ -21228,10 +21225,10 @@
     </row>
     <row r="22" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="110" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="55" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C22" s="51" t="s">
         <v>2</v>
@@ -21288,7 +21285,7 @@
     </row>
     <row r="24" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="49" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B24" s="50"/>
       <c r="C24" s="51"/>
@@ -21344,7 +21341,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C26" s="51" t="s">
         <v>2</v>
@@ -21381,13 +21378,13 @@
         <v>#</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C27" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="61" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E27" s="61" t="s">
         <v>15</v>
@@ -21442,7 +21439,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C29" s="51" t="s">
         <v>2</v>
@@ -21479,7 +21476,7 @@
         <v>#</v>
       </c>
       <c r="B30" s="61" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30" s="64" t="s">
         <v>2</v>
@@ -21516,7 +21513,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C31" s="51" t="s">
         <v>2</v>
@@ -21553,7 +21550,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C32" s="51" t="s">
         <v>2</v>
@@ -21590,7 +21587,7 @@
         <v>#</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C33" s="51" t="s">
         <v>2</v>
@@ -21627,7 +21624,7 @@
         <v>#</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C34" s="51" t="s">
         <v>2</v>
@@ -21664,7 +21661,7 @@
         <v>#</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C35" s="51" t="s">
         <v>2</v>
@@ -21726,7 +21723,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>2</v>
@@ -21763,7 +21760,7 @@
         <v>#</v>
       </c>
       <c r="B38" s="61" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C38" s="64" t="s">
         <v>2</v>
@@ -21800,7 +21797,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="67" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>2</v>
@@ -21837,7 +21834,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="108" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C40" s="51" t="s">
         <v>2</v>
@@ -21872,7 +21869,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="108" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C41" s="51" t="s">
         <v>2</v>
@@ -21907,7 +21904,7 @@
         <v>#</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C42" s="51" t="s">
         <v>2</v>
@@ -21944,7 +21941,7 @@
         <v>#</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C43" s="51" t="s">
         <v>2</v>
@@ -21981,7 +21978,7 @@
         <v>#</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C44" s="51" t="s">
         <v>2</v>
@@ -22039,16 +22036,16 @@
     </row>
     <row r="46" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="110" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C46" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="50" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E46" s="50" t="s">
         <v>22</v>
@@ -22074,16 +22071,16 @@
     </row>
     <row r="47" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B47" s="61" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C47" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="61" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E47" s="61" t="s">
         <v>15</v>
@@ -22109,10 +22106,10 @@
     </row>
     <row r="48" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="110" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B48" s="67" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C48" s="51" t="s">
         <v>2</v>
@@ -22144,10 +22141,10 @@
     </row>
     <row r="49" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="110" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B49" s="67" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C49" s="51" t="s">
         <v>2</v>
@@ -22179,10 +22176,10 @@
     </row>
     <row r="50" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C50" s="51" t="s">
         <v>2</v>
@@ -22214,10 +22211,10 @@
     </row>
     <row r="51" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C51" s="51" t="s">
         <v>2</v>
@@ -22249,10 +22246,10 @@
     </row>
     <row r="52" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C52" s="51" t="s">
         <v>2</v>
@@ -22309,16 +22306,16 @@
     </row>
     <row r="54" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="110" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C54" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E54" s="50" t="s">
         <v>22</v>
@@ -22344,16 +22341,16 @@
     </row>
     <row r="55" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B55" s="61" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C55" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D55" s="61" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E55" s="61" t="s">
         <v>15</v>
@@ -22379,10 +22376,10 @@
     </row>
     <row r="56" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="110" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B56" s="67" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C56" s="51" t="s">
         <v>2</v>
@@ -22414,10 +22411,10 @@
     </row>
     <row r="57" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C57" s="51" t="s">
         <v>2</v>
@@ -22449,10 +22446,10 @@
     </row>
     <row r="58" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B58" s="50" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C58" s="51" t="s">
         <v>2</v>
@@ -22484,10 +22481,10 @@
     </row>
     <row r="59" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B59" s="50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C59" s="51" t="s">
         <v>2</v>
@@ -22544,16 +22541,16 @@
     </row>
     <row r="61" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C61" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D61" s="50" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E61" s="50" t="s">
         <v>22</v>
@@ -22579,16 +22576,16 @@
     </row>
     <row r="62" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B62" s="61" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C62" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="61" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E62" s="61" t="s">
         <v>15</v>
@@ -22639,16 +22636,16 @@
     </row>
     <row r="64" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="110" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B64" s="50" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C64" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D64" s="50" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E64" s="50" t="s">
         <v>22</v>
@@ -22674,16 +22671,16 @@
     </row>
     <row r="65" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="68" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B65" s="69" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C65" s="70" t="s">
         <v>2</v>
       </c>
       <c r="D65" s="69" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E65" s="69" t="s">
         <v>15</v>
@@ -22709,7 +22706,7 @@
     </row>
     <row r="66" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="73" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B66" s="74"/>
       <c r="C66" s="75"/>
@@ -22737,7 +22734,7 @@
     <row r="67" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="78"/>
       <c r="B67" s="74" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C67" s="75" t="s">
         <v>2</v>
@@ -22771,7 +22768,7 @@
     <row r="68" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="78"/>
       <c r="B68" s="74" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C68" s="75" t="s">
         <v>2</v>
@@ -22805,7 +22802,7 @@
     <row r="69" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="78"/>
       <c r="B69" s="74" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C69" s="75" t="s">
         <v>2</v>
@@ -22839,7 +22836,7 @@
     <row r="70" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="78"/>
       <c r="B70" s="74" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C70" s="75" t="s">
         <v>2</v>
@@ -22873,7 +22870,7 @@
     <row r="71" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="78"/>
       <c r="B71" s="74" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C71" s="75" t="s">
         <v>2</v>
@@ -22907,7 +22904,7 @@
     <row r="72" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="78"/>
       <c r="B72" s="74" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C72" s="75" t="s">
         <v>2</v>
@@ -22941,7 +22938,7 @@
     <row r="73" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="78"/>
       <c r="B73" s="74" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C73" s="75" t="s">
         <v>2</v>
@@ -22975,7 +22972,7 @@
     <row r="74" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="79"/>
       <c r="B74" s="80" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C74" s="81" t="s">
         <v>2</v>
@@ -23008,7 +23005,7 @@
     </row>
     <row r="75" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="73" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B75" s="74"/>
       <c r="C75" s="75"/>
@@ -23036,7 +23033,7 @@
     <row r="76" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="78"/>
       <c r="B76" s="74" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C76" s="75" t="s">
         <v>2</v>
@@ -23070,7 +23067,7 @@
     <row r="77" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="78"/>
       <c r="B77" s="74" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C77" s="75" t="s">
         <v>2</v>
@@ -23104,7 +23101,7 @@
     <row r="78" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="78"/>
       <c r="B78" s="74" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C78" s="75" t="s">
         <v>2</v>
@@ -23138,7 +23135,7 @@
     <row r="79" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="79"/>
       <c r="B79" s="80" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C79" s="81" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
modify template for testing of two random experiments
use the same experiment spec twice since idk what else
would be valid... (I'm not a chemist)
</commit_message>
<xml_diff>
--- a/MIT_PVLab_Template.xlsx
+++ b/MIT_PVLab_Template.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="247">
   <si>
     <t>Comment</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>exp1_vols</t>
-  </si>
-  <si>
-    <t>[[500,500]]</t>
   </si>
   <si>
     <t xml:space="preserve">Min and Max volumes for each portion of the experiment. </t>
@@ -1175,9 +1172,6 @@
     <t>Precursor3 (ul)</t>
   </si>
   <si>
-    <t>Precurso4 (ul)</t>
-  </si>
-  <si>
     <t>Precursor5 (ul)</t>
   </si>
   <si>
@@ -1211,13 +1205,7 @@
     <t>Experiment 1 Group Name</t>
   </si>
   <si>
-    <t>Experiment 1</t>
-  </si>
-  <si>
     <t>Experiment 2 Group Name</t>
-  </si>
-  <si>
-    <t>Experiment 2</t>
   </si>
   <si>
     <t>exp1_name</t>
@@ -1226,7 +1214,19 @@
     <t>exp2_name</t>
   </si>
   <si>
-    <t>[[3,1]]</t>
+    <t>Precursor4 (ul)</t>
+  </si>
+  <si>
+    <t>[[215, 215]]</t>
+  </si>
+  <si>
+    <t>qux</t>
+  </si>
+  <si>
+    <t>random_exp1</t>
+  </si>
+  <si>
+    <t>random_exp2</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1820,6 +1820,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2212,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2306,7 +2309,7 @@
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="92" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D3" s="93" t="s">
         <v>2</v>
@@ -2318,7 +2321,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="13"/>
@@ -2350,16 +2353,16 @@
         <v>2</v>
       </c>
       <c r="E4" s="94" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>165</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -2414,13 +2417,13 @@
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="21">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="23" t="s">
@@ -2448,7 +2451,7 @@
     </row>
     <row r="7" spans="1:26" s="32" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="105" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="27"/>
@@ -2482,16 +2485,16 @@
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D8" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G8" s="36" t="s">
         <v>23</v>
@@ -2522,22 +2525,22 @@
       <c r="A9" s="33"/>
       <c r="B9" s="33"/>
       <c r="C9" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D9" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G9" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="37" t="s">
         <v>27</v>
-      </c>
-      <c r="H9" s="37" t="s">
-        <v>28</v>
       </c>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
@@ -2562,22 +2565,22 @@
       <c r="A10" s="33"/>
       <c r="B10" s="33"/>
       <c r="C10" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D10" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10" s="34">
         <v>12</v>
       </c>
       <c r="G10" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="37" t="s">
         <v>30</v>
-      </c>
-      <c r="H10" s="37" t="s">
-        <v>31</v>
       </c>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
@@ -2602,13 +2605,13 @@
       <c r="A11" s="33"/>
       <c r="B11" s="33"/>
       <c r="C11" s="34" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D11" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="36"/>
@@ -2633,8 +2636,8 @@
       <c r="Z11" s="38"/>
     </row>
     <row r="12" spans="1:26" s="32" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="116" t="s">
-        <v>225</v>
+      <c r="A12" s="117" t="s">
+        <v>224</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34"/>
@@ -2663,21 +2666,19 @@
       <c r="Z12" s="38"/>
     </row>
     <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="117" t="s">
-        <v>39</v>
-      </c>
+      <c r="A13" s="118"/>
       <c r="B13" s="33"/>
       <c r="C13" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D13" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>246</v>
+        <v>158</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G13" s="36" t="s">
         <v>23</v>
@@ -2703,24 +2704,22 @@
       <c r="Z13" s="13"/>
     </row>
     <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="117" t="s">
-        <v>39</v>
-      </c>
+      <c r="A14" s="116"/>
       <c r="B14" s="33"/>
       <c r="C14" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D14" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="G14" s="36" t="s">
         <v>26</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>27</v>
       </c>
       <c r="H14" s="37"/>
       <c r="I14" s="13"/>
@@ -2743,24 +2742,22 @@
       <c r="Z14" s="13"/>
     </row>
     <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="117" t="s">
-        <v>39</v>
-      </c>
+      <c r="A15" s="116"/>
       <c r="B15" s="33"/>
       <c r="C15" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D15" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="34">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F15" s="39">
         <v>12</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" s="40"/>
       <c r="I15" s="13"/>
@@ -2783,18 +2780,16 @@
       <c r="Z15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="117" t="s">
-        <v>39</v>
-      </c>
+      <c r="A16" s="118"/>
       <c r="B16" s="33"/>
       <c r="C16" s="34" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D16" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F16" s="39"/>
       <c r="G16" s="36"/>
@@ -2820,7 +2815,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="106" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B17" s="41"/>
       <c r="C17" s="42"/>
@@ -2834,25 +2829,25 @@
       <c r="A18" s="45"/>
       <c r="B18" s="45"/>
       <c r="C18" s="107" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="45" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F18" s="47">
         <v>12</v>
       </c>
       <c r="G18" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H18" s="45"/>
     </row>
     <row r="19" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="49"/>
       <c r="C19" s="50"/>
@@ -2860,10 +2855,10 @@
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
       <c r="G19" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="53" t="s">
         <v>43</v>
-      </c>
-      <c r="H19" s="53" t="s">
-        <v>44</v>
       </c>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
@@ -2887,7 +2882,7 @@
     <row r="20" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
       <c r="B20" s="103" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="51"/>
@@ -2895,7 +2890,7 @@
       <c r="F20" s="50"/>
       <c r="G20" s="52"/>
       <c r="H20" s="60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
@@ -2922,22 +2917,22 @@
         <v>1</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D21" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="114" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F21" s="61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G21" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="62" t="s">
         <v>47</v>
-      </c>
-      <c r="H21" s="62" t="s">
-        <v>48</v>
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
@@ -2960,11 +2955,11 @@
     </row>
     <row r="22" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="109" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="100"/>
       <c r="C22" s="108" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D22" s="51" t="s">
         <v>2</v>
@@ -3026,25 +3021,25 @@
         <v>2</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="96" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F24" s="96" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G24" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="13" t="s">
         <v>161</v>
-      </c>
-      <c r="H24" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
@@ -3066,11 +3061,11 @@
     </row>
     <row r="25" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="101"/>
       <c r="C25" s="50" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D25" s="64" t="s">
         <v>2</v>
@@ -3078,10 +3073,10 @@
       <c r="E25" s="61"/>
       <c r="F25" s="61"/>
       <c r="G25" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="66" t="s">
         <v>51</v>
-      </c>
-      <c r="H25" s="66" t="s">
-        <v>52</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -3106,7 +3101,7 @@
       <c r="A26" s="63"/>
       <c r="B26" s="100"/>
       <c r="C26" s="96" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D26" s="51" t="s">
         <v>2</v>
@@ -3118,10 +3113,10 @@
         <v>3</v>
       </c>
       <c r="G26" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="53" t="s">
         <v>59</v>
-      </c>
-      <c r="H26" s="53" t="s">
-        <v>60</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
@@ -3146,7 +3141,7 @@
       <c r="A27" s="63"/>
       <c r="B27" s="100"/>
       <c r="C27" s="96" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D27" s="51" t="s">
         <v>2</v>
@@ -3158,7 +3153,7 @@
         <v>1.5</v>
       </c>
       <c r="G27" s="52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H27" s="53"/>
       <c r="I27" s="13"/>
@@ -3182,7 +3177,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="104" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B28" s="100"/>
       <c r="C28" s="104"/>
@@ -3212,11 +3207,11 @@
     </row>
     <row r="29" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" s="100"/>
       <c r="C29" s="50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D29" s="51" t="s">
         <v>2</v>
@@ -3228,10 +3223,10 @@
         <v>75</v>
       </c>
       <c r="G29" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" s="53" t="s">
         <v>64</v>
-      </c>
-      <c r="H29" s="53" t="s">
-        <v>65</v>
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
@@ -3254,11 +3249,11 @@
     </row>
     <row r="30" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="100"/>
       <c r="C30" s="50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D30" s="51" t="s">
         <v>2</v>
@@ -3270,10 +3265,10 @@
         <v>450</v>
       </c>
       <c r="G30" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H30" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
@@ -3296,11 +3291,11 @@
     </row>
     <row r="31" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="100"/>
       <c r="C31" s="50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D31" s="51" t="s">
         <v>2</v>
@@ -3312,10 +3307,10 @@
         <v>3600</v>
       </c>
       <c r="G31" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H31" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
@@ -3370,19 +3365,19 @@
         <v>3</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D33" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E33" s="96" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F33" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="G33" s="52" t="s">
         <v>71</v>
-      </c>
-      <c r="G33" s="52" t="s">
-        <v>72</v>
       </c>
       <c r="H33" s="53"/>
       <c r="I33" s="13"/>
@@ -3406,24 +3401,24 @@
     </row>
     <row r="34" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="101"/>
       <c r="C34" s="108" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D34" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E34" s="61"/>
       <c r="F34" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G34" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="66" t="s">
         <v>51</v>
-      </c>
-      <c r="H34" s="66" t="s">
-        <v>52</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
@@ -3448,7 +3443,7 @@
       <c r="A35" s="63"/>
       <c r="B35" s="100"/>
       <c r="C35" s="50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D35" s="51" t="s">
         <v>2</v>
@@ -3460,7 +3455,7 @@
         <v>6</v>
       </c>
       <c r="G35" s="52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H35" s="53"/>
       <c r="I35" s="13"/>
@@ -3486,7 +3481,7 @@
       <c r="A36" s="63"/>
       <c r="B36" s="100"/>
       <c r="C36" s="50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D36" s="51" t="s">
         <v>2</v>
@@ -3520,7 +3515,7 @@
       <c r="A37" s="63"/>
       <c r="B37" s="100"/>
       <c r="C37" s="50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D37" s="51" t="s">
         <v>2</v>
@@ -3552,7 +3547,7 @@
     </row>
     <row r="38" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="104" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B38" s="100"/>
       <c r="C38" s="50"/>
@@ -3582,11 +3577,11 @@
     </row>
     <row r="39" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="100"/>
       <c r="C39" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D39" s="51" t="s">
         <v>2</v>
@@ -3598,10 +3593,10 @@
         <v>75</v>
       </c>
       <c r="G39" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="H39" s="53" t="s">
         <v>64</v>
-      </c>
-      <c r="H39" s="53" t="s">
-        <v>65</v>
       </c>
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
@@ -3624,11 +3619,11 @@
     </row>
     <row r="40" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="100"/>
       <c r="C40" s="50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D40" s="51" t="s">
         <v>2</v>
@@ -3640,10 +3635,10 @@
         <v>450</v>
       </c>
       <c r="G40" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H40" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
@@ -3666,11 +3661,11 @@
     </row>
     <row r="41" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="100"/>
       <c r="C41" s="50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D41" s="51" t="s">
         <v>2</v>
@@ -3682,10 +3677,10 @@
         <v>3600</v>
       </c>
       <c r="G41" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H41" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
@@ -3736,23 +3731,23 @@
     </row>
     <row r="43" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" s="100">
         <v>4</v>
       </c>
       <c r="C43" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D43" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E43" s="50"/>
       <c r="F43" s="50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G43" s="52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H43" s="56"/>
       <c r="I43" s="13"/>
@@ -3776,24 +3771,24 @@
     </row>
     <row r="44" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="101"/>
       <c r="C44" s="108" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D44" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E44" s="61"/>
       <c r="F44" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G44" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H44" s="66" t="s">
         <v>51</v>
-      </c>
-      <c r="H44" s="66" t="s">
-        <v>52</v>
       </c>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
@@ -3816,11 +3811,11 @@
     </row>
     <row r="45" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" s="100"/>
       <c r="C45" s="50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D45" s="51" t="s">
         <v>2</v>
@@ -3830,7 +3825,7 @@
         <v>2</v>
       </c>
       <c r="G45" s="52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H45" s="53"/>
       <c r="I45" s="13"/>
@@ -3854,11 +3849,11 @@
     </row>
     <row r="46" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="100"/>
       <c r="C46" s="50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D46" s="51" t="s">
         <v>2</v>
@@ -3868,7 +3863,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H46" s="53"/>
       <c r="I46" s="13"/>
@@ -3892,11 +3887,11 @@
     </row>
     <row r="47" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="100"/>
       <c r="C47" s="50" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D47" s="51" t="s">
         <v>2</v>
@@ -3908,10 +3903,10 @@
         <v>75</v>
       </c>
       <c r="G47" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="H47" s="53" t="s">
         <v>64</v>
-      </c>
-      <c r="H47" s="53" t="s">
-        <v>65</v>
       </c>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
@@ -3934,11 +3929,11 @@
     </row>
     <row r="48" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="100"/>
       <c r="C48" s="50" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D48" s="51" t="s">
         <v>2</v>
@@ -3950,10 +3945,10 @@
         <v>450</v>
       </c>
       <c r="G48" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H48" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
@@ -3976,11 +3971,11 @@
     </row>
     <row r="49" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B49" s="100"/>
       <c r="C49" s="50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D49" s="51" t="s">
         <v>2</v>
@@ -3992,10 +3987,10 @@
         <v>3600</v>
       </c>
       <c r="G49" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H49" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
@@ -4046,23 +4041,23 @@
     </row>
     <row r="51" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B51" s="100">
         <v>5</v>
       </c>
       <c r="C51" s="50" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D51" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E51" s="50"/>
       <c r="F51" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G51" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H51" s="53"/>
       <c r="I51" s="13"/>
@@ -4086,24 +4081,24 @@
     </row>
     <row r="52" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B52" s="101"/>
       <c r="C52" s="61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D52" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E52" s="61"/>
       <c r="F52" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G52" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H52" s="66" t="s">
         <v>51</v>
-      </c>
-      <c r="H52" s="66" t="s">
-        <v>52</v>
       </c>
       <c r="I52" s="13"/>
       <c r="J52" s="13"/>
@@ -4126,11 +4121,11 @@
     </row>
     <row r="53" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B53" s="101"/>
       <c r="C53" s="50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D53" s="51" t="s">
         <v>2</v>
@@ -4160,11 +4155,11 @@
     </row>
     <row r="54" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B54" s="101"/>
       <c r="C54" s="50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D54" s="51" t="s">
         <v>2</v>
@@ -4194,11 +4189,11 @@
     </row>
     <row r="55" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B55" s="101"/>
       <c r="C55" s="50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D55" s="51" t="s">
         <v>2</v>
@@ -4208,7 +4203,7 @@
         <v>4.5</v>
       </c>
       <c r="G55" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H55" s="56"/>
       <c r="I55" s="13"/>
@@ -4232,11 +4227,11 @@
     </row>
     <row r="56" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" s="101"/>
       <c r="C56" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D56" s="51" t="s">
         <v>2</v>
@@ -4248,10 +4243,10 @@
         <v>75</v>
       </c>
       <c r="G56" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="H56" s="53" t="s">
         <v>64</v>
-      </c>
-      <c r="H56" s="53" t="s">
-        <v>65</v>
       </c>
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
@@ -4274,11 +4269,11 @@
     </row>
     <row r="57" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57" s="101"/>
       <c r="C57" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D57" s="51" t="s">
         <v>2</v>
@@ -4290,10 +4285,10 @@
         <v>450</v>
       </c>
       <c r="G57" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H57" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
@@ -4316,11 +4311,11 @@
     </row>
     <row r="58" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B58" s="101"/>
       <c r="C58" s="50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D58" s="51" t="s">
         <v>2</v>
@@ -4332,10 +4327,10 @@
         <v>3600</v>
       </c>
       <c r="G58" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H58" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
@@ -4386,23 +4381,23 @@
     </row>
     <row r="60" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B60" s="100">
         <v>6</v>
       </c>
       <c r="C60" s="50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D60" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E60" s="50"/>
       <c r="F60" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="G60" s="52" t="s">
         <v>101</v>
-      </c>
-      <c r="G60" s="52" t="s">
-        <v>102</v>
       </c>
       <c r="H60" s="53"/>
       <c r="I60" s="13"/>
@@ -4431,7 +4426,7 @@
       </c>
       <c r="B61" s="100"/>
       <c r="C61" s="50" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D61" s="51"/>
       <c r="E61" s="50"/>
@@ -4464,20 +4459,20 @@
       </c>
       <c r="B62" s="101"/>
       <c r="C62" s="61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D62" s="64" t="s">
         <v>2</v>
       </c>
       <c r="E62" s="61"/>
       <c r="F62" s="61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G62" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H62" s="66" t="s">
         <v>51</v>
-      </c>
-      <c r="H62" s="66" t="s">
-        <v>52</v>
       </c>
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
@@ -4528,23 +4523,23 @@
     </row>
     <row r="64" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B64" s="100">
         <v>7</v>
       </c>
       <c r="C64" s="50" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D64" s="51" t="s">
         <v>2</v>
       </c>
       <c r="E64" s="50"/>
       <c r="F64" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="G64" s="52" t="s">
         <v>101</v>
-      </c>
-      <c r="G64" s="52" t="s">
-        <v>102</v>
       </c>
       <c r="H64" s="53"/>
       <c r="I64" s="13"/>
@@ -4573,7 +4568,7 @@
       </c>
       <c r="B65" s="100"/>
       <c r="C65" s="50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D65" s="97" t="s">
         <v>2</v>
@@ -4631,13 +4626,13 @@
     </row>
     <row r="67" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B67" s="100">
         <v>8</v>
       </c>
       <c r="C67" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D67" s="97" t="s">
         <v>2</v>
@@ -4672,7 +4667,7 @@
       </c>
       <c r="B68" s="102"/>
       <c r="C68" s="69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D68" s="98" t="s">
         <v>2</v>
@@ -4702,7 +4697,7 @@
     </row>
     <row r="69" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="99" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B69" s="99"/>
       <c r="C69" s="74"/>
@@ -4734,7 +4729,7 @@
       <c r="A70" s="78"/>
       <c r="B70" s="78"/>
       <c r="C70" s="74" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D70" s="75" t="s">
         <v>2</v>
@@ -4746,7 +4741,7 @@
         <v>750</v>
       </c>
       <c r="G70" s="76" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H70" s="77"/>
       <c r="I70" s="13"/>
@@ -4772,7 +4767,7 @@
       <c r="A71" s="78"/>
       <c r="B71" s="78"/>
       <c r="C71" s="74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D71" s="75" t="s">
         <v>2</v>
@@ -4784,7 +4779,7 @@
         <v>80</v>
       </c>
       <c r="G71" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H71" s="77"/>
       <c r="I71" s="13"/>
@@ -4810,7 +4805,7 @@
       <c r="A72" s="78"/>
       <c r="B72" s="78"/>
       <c r="C72" s="74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D72" s="75" t="s">
         <v>2</v>
@@ -4822,7 +4817,7 @@
         <v>900</v>
       </c>
       <c r="G72" s="76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H72" s="77"/>
       <c r="I72" s="13"/>
@@ -4848,7 +4843,7 @@
       <c r="A73" s="78"/>
       <c r="B73" s="78"/>
       <c r="C73" s="74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D73" s="75" t="s">
         <v>2</v>
@@ -4860,7 +4855,7 @@
         <v>1200</v>
       </c>
       <c r="G73" s="76" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H73" s="77"/>
       <c r="I73" s="13"/>
@@ -4886,7 +4881,7 @@
       <c r="A74" s="78"/>
       <c r="B74" s="78"/>
       <c r="C74" s="74" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D74" s="75" t="s">
         <v>2</v>
@@ -4898,10 +4893,10 @@
         <v>105</v>
       </c>
       <c r="G74" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="H74" s="77" t="s">
         <v>117</v>
-      </c>
-      <c r="H74" s="77" t="s">
-        <v>118</v>
       </c>
       <c r="I74" s="13"/>
       <c r="J74" s="13"/>
@@ -4926,7 +4921,7 @@
       <c r="A75" s="78"/>
       <c r="B75" s="78"/>
       <c r="C75" s="74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D75" s="75" t="s">
         <v>2</v>
@@ -4938,10 +4933,10 @@
         <v>12600</v>
       </c>
       <c r="G75" s="76" t="s">
+        <v>119</v>
+      </c>
+      <c r="H75" s="77" t="s">
         <v>120</v>
-      </c>
-      <c r="H75" s="77" t="s">
-        <v>121</v>
       </c>
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
@@ -4966,7 +4961,7 @@
       <c r="A76" s="78"/>
       <c r="B76" s="78"/>
       <c r="C76" s="74" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D76" s="75" t="s">
         <v>2</v>
@@ -4978,10 +4973,10 @@
         <v>3</v>
       </c>
       <c r="G76" s="76" t="s">
+        <v>122</v>
+      </c>
+      <c r="H76" s="77" t="s">
         <v>123</v>
-      </c>
-      <c r="H76" s="77" t="s">
-        <v>124</v>
       </c>
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
@@ -5004,24 +4999,24 @@
     </row>
     <row r="77" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B77" s="79"/>
       <c r="C77" s="80" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D77" s="81" t="s">
         <v>2</v>
       </c>
       <c r="E77" s="111" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F77" s="80"/>
       <c r="G77" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="H77" s="83" t="s">
         <v>126</v>
-      </c>
-      <c r="H77" s="83" t="s">
-        <v>127</v>
       </c>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
@@ -5044,7 +5039,7 @@
     </row>
     <row r="78" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="99" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B78" s="99"/>
       <c r="C78" s="74"/>
@@ -5076,7 +5071,7 @@
       <c r="A79" s="78"/>
       <c r="B79" s="78"/>
       <c r="C79" s="112" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D79" s="75" t="s">
         <v>2</v>
@@ -5088,10 +5083,10 @@
         <v>45</v>
       </c>
       <c r="G79" s="113" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H79" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I79" s="13"/>
       <c r="J79" s="13"/>
@@ -5116,7 +5111,7 @@
       <c r="A80" s="78"/>
       <c r="B80" s="78"/>
       <c r="C80" s="74" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D80" s="75" t="s">
         <v>2</v>
@@ -5128,10 +5123,10 @@
         <v>75</v>
       </c>
       <c r="G80" s="76" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H80" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I80" s="13"/>
       <c r="J80" s="13"/>
@@ -5156,7 +5151,7 @@
       <c r="A81" s="78"/>
       <c r="B81" s="78"/>
       <c r="C81" s="74" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D81" s="75" t="s">
         <v>2</v>
@@ -5168,10 +5163,10 @@
         <v>450</v>
       </c>
       <c r="G81" s="76" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H81" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I81" s="13"/>
       <c r="J81" s="13"/>
@@ -5196,7 +5191,7 @@
       <c r="A82" s="79"/>
       <c r="B82" s="79"/>
       <c r="C82" s="80" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D82" s="81" t="s">
         <v>2</v>
@@ -5208,10 +5203,10 @@
         <v>3600</v>
       </c>
       <c r="G82" s="82" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H82" s="83" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
@@ -14423,7 +14418,7 @@
       <c r="H1001" s="88"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" promptTitle="Experiment Count" prompt="MUST be the sum of &quot;Random Experiments&quot; and &quot;Manual Experiments&quot;" sqref="E6">
       <formula1>SUM(#REF!,E18)</formula1>
     </dataValidation>
@@ -14442,7 +14437,7 @@
   <dimension ref="A1:T500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14456,37 +14451,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="89" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C1" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="89" t="s">
         <v>226</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="E1" s="89" t="s">
         <v>227</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="F1" s="89" t="s">
+        <v>242</v>
+      </c>
+      <c r="G1" s="89" t="s">
         <v>228</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="H1" s="89" t="s">
         <v>229</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="I1" s="89" t="s">
         <v>230</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="J1" s="90" t="s">
         <v>231</v>
       </c>
-      <c r="I1" s="89" t="s">
+      <c r="K1" s="90" t="s">
         <v>232</v>
-      </c>
-      <c r="J1" s="90" t="s">
-        <v>233</v>
-      </c>
-      <c r="K1" s="90" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
@@ -14495,7 +14490,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="91" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C2" s="90">
         <v>150</v>
@@ -14532,7 +14527,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C3" s="90">
         <v>150</v>
@@ -14569,7 +14564,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="91" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C4" s="90">
         <v>150</v>
@@ -14601,14 +14596,40 @@
       </c>
     </row>
     <row r="5" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="91" t="str">
+      <c r="A5" s="91">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B5" s="91"/>
-      <c r="K5" s="90" t="str">
+        <v>4</v>
+      </c>
+      <c r="B5" s="91" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="90">
+        <v>150</v>
+      </c>
+      <c r="D5" s="90">
+        <v>30</v>
+      </c>
+      <c r="E5" s="90">
+        <v>35</v>
+      </c>
+      <c r="F5" s="90">
+        <v>0</v>
+      </c>
+      <c r="G5" s="90">
+        <v>0</v>
+      </c>
+      <c r="H5" s="90">
+        <v>0</v>
+      </c>
+      <c r="I5" s="90">
+        <v>0</v>
+      </c>
+      <c r="J5" s="90">
+        <v>0</v>
+      </c>
+      <c r="K5" s="90">
         <f t="shared" si="0"/>
-        <v/>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="90" customFormat="1" x14ac:dyDescent="0.2">
@@ -16040,7 +16061,7 @@
   <dimension ref="A1:K98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16052,37 +16073,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="89" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="89" t="s">
-        <v>235</v>
-      </c>
-      <c r="C1" s="89" t="s">
+      <c r="D1" s="89" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="E1" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="F1" s="89" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="G1" s="89" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="H1" s="89" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="I1" s="89" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="89" t="s">
-        <v>144</v>
-      </c>
       <c r="J1" s="89" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K1" s="90" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -16224,49 +16245,49 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
+      <c r="A5">
         <f>IF(NOT('Manual Experiment Interface'!A5=""),'Manual Experiment Interface'!A5,"")</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="B5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B5=""),'Manual Experiment Interface'!B5,"")</f>
-        <v/>
-      </c>
-      <c r="C5" t="str">
+        <v>qux</v>
+      </c>
+      <c r="C5">
         <f>IF(NOT('Manual Experiment Interface'!C5=""),'Manual Experiment Interface'!C5,"")</f>
-        <v/>
-      </c>
-      <c r="D5" t="str">
+        <v>150</v>
+      </c>
+      <c r="D5">
         <f>IF(NOT('Manual Experiment Interface'!D5=""),'Manual Experiment Interface'!D5,"")</f>
-        <v/>
-      </c>
-      <c r="E5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E5">
         <f>IF(NOT('Manual Experiment Interface'!E5=""),'Manual Experiment Interface'!E5,"")</f>
-        <v/>
-      </c>
-      <c r="F5" t="str">
+        <v>35</v>
+      </c>
+      <c r="F5">
         <f>IF(NOT('Manual Experiment Interface'!F5=""),'Manual Experiment Interface'!F5,"")</f>
-        <v/>
-      </c>
-      <c r="G5" t="str">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <f>IF(NOT('Manual Experiment Interface'!G5=""),'Manual Experiment Interface'!G5,"")</f>
-        <v/>
-      </c>
-      <c r="H5" t="str">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <f>IF(NOT('Manual Experiment Interface'!H5=""),'Manual Experiment Interface'!H5,"")</f>
-        <v/>
-      </c>
-      <c r="I5" t="str">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <f>IF(NOT('Manual Experiment Interface'!I5=""),'Manual Experiment Interface'!I5,"")</f>
-        <v/>
-      </c>
-      <c r="J5" t="str">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <f>IF(NOT('Manual Experiment Interface'!J5=""),'Manual Experiment Interface'!J5,"")</f>
-        <v/>
-      </c>
-      <c r="K5" t="str">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <f>IF(NOT('Manual Experiment Interface'!K5=""),'Manual Experiment Interface'!K5,"")</f>
-        <v/>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -20556,8 +20577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W998"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20770,7 +20791,7 @@
       </c>
       <c r="D7" s="21">
         <f>'User Interface'!wellcount</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>12</v>
@@ -20901,14 +20922,14 @@
         <v>0</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="34">
         <f>'User Interface'!E10</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>12</v>
@@ -20938,14 +20959,14 @@
         <v>0</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C12" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="34" t="str">
         <f>'User Interface'!E11</f>
-        <v>Experiment 1</v>
+        <v>random_exp1</v>
       </c>
       <c r="E12" s="34"/>
       <c r="F12" s="38"/>
@@ -20968,19 +20989,19 @@
       <c r="W12" s="38"/>
     </row>
     <row r="13" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="str">
+      <c r="A13" s="33">
         <f>'User Interface'!A13</f>
-        <v>#</v>
+        <v>0</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="34" t="str">
         <f>'User Interface'!E13</f>
-        <v>[[3,1]]</v>
+        <v>[[2,3,1]]</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>22</v>
@@ -21005,19 +21026,19 @@
       <c r="W13" s="13"/>
     </row>
     <row r="14" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="str">
+      <c r="A14" s="33">
         <f>'User Interface'!A14</f>
-        <v>#</v>
+        <v>0</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="34" t="str">
         <f>'User Interface'!E14</f>
-        <v>[[500,500]]</v>
+        <v>[[215, 215]]</v>
       </c>
       <c r="E14" s="34" t="s">
         <v>22</v>
@@ -21042,19 +21063,19 @@
       <c r="W14" s="13"/>
     </row>
     <row r="15" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="str">
+      <c r="A15" s="33">
         <f>'User Interface'!A15</f>
-        <v>#</v>
+        <v>0</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="34">
         <f>'User Interface'!E15</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E15" s="34" t="s">
         <v>12</v>
@@ -21079,19 +21100,19 @@
       <c r="W15" s="13"/>
     </row>
     <row r="16" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="str">
+      <c r="A16" s="33">
         <f>'User Interface'!A16</f>
-        <v>#</v>
+        <v>0</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="34" t="str">
         <f>'User Interface'!E16</f>
-        <v>Experiment 2</v>
+        <v>random_exp2</v>
       </c>
       <c r="E16" s="34"/>
       <c r="F16" s="13"/>
@@ -21115,7 +21136,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
@@ -21125,12 +21146,12 @@
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="45"/>
       <c r="B18" s="45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="45"/>
       <c r="D18" s="34">
         <f>'User Interface'!E18</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18" s="45" t="s">
         <v>12</v>
@@ -21138,7 +21159,7 @@
     </row>
     <row r="19" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="50"/>
       <c r="C19" s="51"/>
@@ -21190,10 +21211,10 @@
     </row>
     <row r="21" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="55" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" s="55" t="s">
-        <v>40</v>
       </c>
       <c r="C21" s="51" t="s">
         <v>2</v>
@@ -21225,10 +21246,10 @@
     </row>
     <row r="22" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="51" t="s">
         <v>2</v>
@@ -21285,7 +21306,7 @@
     </row>
     <row r="24" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="50"/>
       <c r="C24" s="51"/>
@@ -21341,7 +21362,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="51" t="s">
         <v>2</v>
@@ -21378,13 +21399,13 @@
         <v>#</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="61" t="s">
         <v>15</v>
@@ -21439,7 +21460,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="51" t="s">
         <v>2</v>
@@ -21476,7 +21497,7 @@
         <v>#</v>
       </c>
       <c r="B30" s="61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="64" t="s">
         <v>2</v>
@@ -21513,7 +21534,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="51" t="s">
         <v>2</v>
@@ -21550,7 +21571,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="51" t="s">
         <v>2</v>
@@ -21587,7 +21608,7 @@
         <v>#</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="51" t="s">
         <v>2</v>
@@ -21624,7 +21645,7 @@
         <v>#</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="51" t="s">
         <v>2</v>
@@ -21661,7 +21682,7 @@
         <v>#</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="51" t="s">
         <v>2</v>
@@ -21723,7 +21744,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>2</v>
@@ -21760,7 +21781,7 @@
         <v>#</v>
       </c>
       <c r="B38" s="61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="64" t="s">
         <v>2</v>
@@ -21797,7 +21818,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>2</v>
@@ -21834,7 +21855,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="108" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C40" s="51" t="s">
         <v>2</v>
@@ -21869,7 +21890,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="108" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C41" s="51" t="s">
         <v>2</v>
@@ -21904,7 +21925,7 @@
         <v>#</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="51" t="s">
         <v>2</v>
@@ -21941,7 +21962,7 @@
         <v>#</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" s="51" t="s">
         <v>2</v>
@@ -21978,7 +21999,7 @@
         <v>#</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="51" t="s">
         <v>2</v>
@@ -22036,16 +22057,16 @@
     </row>
     <row r="46" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E46" s="50" t="s">
         <v>22</v>
@@ -22071,16 +22092,16 @@
     </row>
     <row r="47" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E47" s="61" t="s">
         <v>15</v>
@@ -22106,10 +22127,10 @@
     </row>
     <row r="48" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="51" t="s">
         <v>2</v>
@@ -22141,10 +22162,10 @@
     </row>
     <row r="49" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B49" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" s="51" t="s">
         <v>2</v>
@@ -22176,10 +22197,10 @@
     </row>
     <row r="50" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="51" t="s">
         <v>2</v>
@@ -22211,10 +22232,10 @@
     </row>
     <row r="51" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" s="51" t="s">
         <v>2</v>
@@ -22246,10 +22267,10 @@
     </row>
     <row r="52" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C52" s="51" t="s">
         <v>2</v>
@@ -22306,16 +22327,16 @@
     </row>
     <row r="54" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C54" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E54" s="50" t="s">
         <v>22</v>
@@ -22341,16 +22362,16 @@
     </row>
     <row r="55" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B55" s="61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C55" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D55" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E55" s="61" t="s">
         <v>15</v>
@@ -22376,10 +22397,10 @@
     </row>
     <row r="56" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" s="67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C56" s="51" t="s">
         <v>2</v>
@@ -22411,10 +22432,10 @@
     </row>
     <row r="57" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C57" s="51" t="s">
         <v>2</v>
@@ -22446,10 +22467,10 @@
     </row>
     <row r="58" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B58" s="50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C58" s="51" t="s">
         <v>2</v>
@@ -22481,10 +22502,10 @@
     </row>
     <row r="59" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B59" s="50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C59" s="51" t="s">
         <v>2</v>
@@ -22541,16 +22562,16 @@
     </row>
     <row r="61" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C61" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D61" s="50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E61" s="50" t="s">
         <v>22</v>
@@ -22576,16 +22597,16 @@
     </row>
     <row r="62" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62" s="61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C62" s="64" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E62" s="61" t="s">
         <v>15</v>
@@ -22636,16 +22657,16 @@
     </row>
     <row r="64" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="110" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B64" s="50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C64" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D64" s="50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E64" s="50" t="s">
         <v>22</v>
@@ -22671,16 +22692,16 @@
     </row>
     <row r="65" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="68" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B65" s="69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C65" s="70" t="s">
         <v>2</v>
       </c>
       <c r="D65" s="69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E65" s="69" t="s">
         <v>15</v>
@@ -22706,7 +22727,7 @@
     </row>
     <row r="66" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B66" s="74"/>
       <c r="C66" s="75"/>
@@ -22734,7 +22755,7 @@
     <row r="67" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="78"/>
       <c r="B67" s="74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C67" s="75" t="s">
         <v>2</v>
@@ -22768,7 +22789,7 @@
     <row r="68" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="78"/>
       <c r="B68" s="74" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C68" s="75" t="s">
         <v>2</v>
@@ -22802,7 +22823,7 @@
     <row r="69" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="78"/>
       <c r="B69" s="74" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C69" s="75" t="s">
         <v>2</v>
@@ -22836,7 +22857,7 @@
     <row r="70" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="78"/>
       <c r="B70" s="74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C70" s="75" t="s">
         <v>2</v>
@@ -22870,7 +22891,7 @@
     <row r="71" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="78"/>
       <c r="B71" s="74" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C71" s="75" t="s">
         <v>2</v>
@@ -22904,7 +22925,7 @@
     <row r="72" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="78"/>
       <c r="B72" s="74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C72" s="75" t="s">
         <v>2</v>
@@ -22938,7 +22959,7 @@
     <row r="73" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="78"/>
       <c r="B73" s="74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C73" s="75" t="s">
         <v>2</v>
@@ -22972,7 +22993,7 @@
     <row r="74" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="79"/>
       <c r="B74" s="80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C74" s="81" t="s">
         <v>2</v>
@@ -23005,7 +23026,7 @@
     </row>
     <row r="75" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B75" s="74"/>
       <c r="C75" s="75"/>
@@ -23033,7 +23054,7 @@
     <row r="76" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="78"/>
       <c r="B76" s="74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C76" s="75" t="s">
         <v>2</v>
@@ -23067,7 +23088,7 @@
     <row r="77" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="78"/>
       <c r="B77" s="74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C77" s="75" t="s">
         <v>2</v>
@@ -23101,7 +23122,7 @@
     <row r="78" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="78"/>
       <c r="B78" s="74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C78" s="75" t="s">
         <v>2</v>
@@ -23135,7 +23156,7 @@
     <row r="79" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="79"/>
       <c r="B79" s="80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C79" s="81" t="s">
         <v>2</v>

</xml_diff>